<commit_message>
Keyword Driven framework  With Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/kw_scripts/ShiftVisionKeywordTest.xlsx
+++ b/src/test/resources/kw_scripts/ShiftVisionKeywordTest.xlsx
@@ -3,7 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Login01" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TestScript" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Login01" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Login02" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Login03" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,12 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>TestScriptDescription</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Valid login with valid password</t>
+  </si>
+  <si>
+    <t>Login01</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Valid login with invalid password</t>
+  </si>
+  <si>
+    <t>Login02</t>
+  </si>
+  <si>
+    <t>InValid login with valid password</t>
+  </si>
+  <si>
+    <t>Login03</t>
+  </si>
   <si>
     <t>Step</t>
   </si>
   <si>
-    <t>Descriptiopn</t>
+    <t>Description</t>
   </si>
   <si>
     <t>Keyword</t>
@@ -89,6 +125,27 @@
   </si>
   <si>
     <t>CLOSE_BROWSER</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>Wait 2 sec</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
+    <t>Verify login error message</t>
+  </si>
+  <si>
+    <t>XPATH://form/p</t>
+  </si>
+  <si>
+    <t>The e-mail address and/or password entered do not match our records. Please try again.</t>
+  </si>
+  <si>
+    <t>invalid@shiftvision.com</t>
   </si>
 </sst>
 </file>
@@ -152,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -165,9 +222,13 @@
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -178,6 +239,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -385,6 +458,81 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="2.38"/>
+    <col customWidth="1" min="2" max="2" width="29.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="1" max="1" width="6.25"/>
     <col customWidth="1" min="2" max="2" width="33.5"/>
     <col customWidth="1" min="3" max="3" width="21.75"/>
@@ -394,19 +542,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -414,14 +562,14 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -429,31 +577,31 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="2">
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -461,16 +609,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -478,31 +626,31 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -510,13 +658,345 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.25"/>
+    <col customWidth="1" min="2" max="2" width="33.5"/>
+    <col customWidth="1" min="3" max="3" width="21.75"/>
+    <col customWidth="1" min="4" max="4" width="30.75"/>
+    <col customWidth="1" min="5" max="5" width="69.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7">
+        <v>2000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.25"/>
+    <col customWidth="1" min="2" max="2" width="33.5"/>
+    <col customWidth="1" min="3" max="3" width="21.75"/>
+    <col customWidth="1" min="4" max="4" width="30.75"/>
+    <col customWidth="1" min="5" max="5" width="69.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7">
+        <v>2000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>